<commit_message>
Status update and Employee/owner details in new page
</commit_message>
<xml_diff>
--- a/upload/نموذج أضافة المبانى -أمان.xlsx
+++ b/upload/نموذج أضافة المبانى -أمان.xlsx
@@ -1,17 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jainc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spsa\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2161555-01DA-4123-B3DD-87D3681AACD2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="KBWrCCxOEe/jWucySwJkboDyZQi18Dyfoykg47daGOjtBa80FYhtMfSsMOFeWncwQIvjlN0p5Wv73D7pCPYeAQ==" workbookSaltValue="p9Zg1/BxgQjgwb2Y6W+HaQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="450" windowWidth="14505" windowHeight="10350" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="التعليمات " sheetId="1" r:id="rId1"/>
@@ -27,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>a</t>
   </si>
@@ -50,9 +48,6 @@
     <t xml:space="preserve">رقم المبنى </t>
   </si>
   <si>
-    <t xml:space="preserve">شارع المبنى </t>
-  </si>
-  <si>
     <t xml:space="preserve">رقم قطعة الارض </t>
   </si>
   <si>
@@ -62,9 +57,6 @@
     <t xml:space="preserve">رقم الهاتف البديل للتواصل 2 </t>
   </si>
   <si>
-    <t xml:space="preserve">جدول المفضل </t>
-  </si>
-  <si>
     <t xml:space="preserve">أدخل اسم المبنى </t>
   </si>
   <si>
@@ -80,9 +72,6 @@
     <t xml:space="preserve">ملاحظات </t>
   </si>
   <si>
-    <t>مالك المبنى هو الوحيد المصرح له بتحميل النموذج المعبأ.</t>
-  </si>
-  <si>
     <t xml:space="preserve">رقم </t>
   </si>
   <si>
@@ -107,77 +96,35 @@
     <t>يتم الابلاغ عن أي مشاكل في التحميل على الفور.</t>
   </si>
   <si>
-    <t xml:space="preserve"> ادخل جدولك المفضل بالسنة / اليوم / الشهر والوقت لتنسيق</t>
-  </si>
-  <si>
     <t>عملية التحميل لا تضمن التثبيت او اى اتصالات من مركز الاتصال حتى تقوم انت بطلب الخدمة .</t>
   </si>
   <si>
     <t>بموجرد ملئ النموذج وتحميلة ،تحتاج للنقر فوق طلب الخدمة لتثبيت جهاز لوحه تحكم انذار الحريق</t>
   </si>
   <si>
-    <t>عزيزى مالك المبنى ,                                                                                                                                                               يجب تحميل النموذج من قائمة المبانى التى تطلب تثبيت جهاز لوحه تحكم أنذار الحريق من خلال هذا النموذج بصرف النظر عن عدد المبانى وعناوينها ،يمكنك ايضا توفير رقمين بديلين لاتصال بة يمكن الوصول اليهما فى حالة غيابك اثناء إجراء التثبيت أو لإى استفسارات من هذا القبيل من قبل مركز الاتصال .</t>
-  </si>
-  <si>
-    <t>Building Name</t>
-  </si>
-  <si>
-    <t>Building No</t>
-  </si>
-  <si>
-    <t>Building Street</t>
-  </si>
-  <si>
-    <t>Plot No</t>
-  </si>
-  <si>
-    <t>Alternate Contact Phone Number 1</t>
-  </si>
-  <si>
-    <t>Alternate Contact Phone Number 2</t>
-  </si>
-  <si>
-    <t>Preferred Schedule</t>
-  </si>
-  <si>
-    <t>مبنى الفردان</t>
-  </si>
-  <si>
-    <t>مبنى 784567</t>
-  </si>
-  <si>
-    <t>شارع الزهراء</t>
-  </si>
-  <si>
-    <t>مبنى الروية</t>
-  </si>
-  <si>
-    <t>مبنى 893939</t>
-  </si>
-  <si>
-    <t>ابو شغارة</t>
-  </si>
-  <si>
-    <t>20-04-19</t>
-  </si>
-  <si>
-    <t>الفيحاء</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> مبنى 893499</t>
-  </si>
-  <si>
-    <t>مبنى المروان</t>
-  </si>
-  <si>
-    <t>april-25-19</t>
+    <t>عزيزى مالك المبنى ,                                                                                                                                                               يجب تحميل النموذج من قائمة المبانى التى تطلب تثبيت جهاز لوحه تحكم أنذار الحريق من خلال هذا النموذج بصرف النظر عن عدد المبانى وعناوينها ،يمكنك ايضا توفير رقمين بديلين لاتصال وذلك للوصول اليهما فى حالة غيابك اثناء إجراء التثبيت أو لإى استفسارات من هذا القبيل من قبل مركز الاتصال .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">الشارع </t>
+  </si>
+  <si>
+    <t>جدول التركيب</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ادخل تأريخ المفضل بالسنة / اليوم / الشهر والوقت لتنسيق</t>
+  </si>
+  <si>
+    <t>مالك المبنى هو الوحيد أو من ينوب عنه المصرح له بتحميل النموذج المعبأ.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">جدول التركيب </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,16 +171,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF212121"/>
-      <name val="Inherit"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF212121"/>
-      <name val="Inherit"/>
     </font>
   </fonts>
   <fills count="3">
@@ -296,7 +233,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -332,12 +269,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
@@ -355,13 +286,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -436,23 +360,23 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>225136</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>51954</xdr:rowOff>
+      <xdr:colOff>233795</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>173182</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1723158</xdr:colOff>
+      <xdr:colOff>1757795</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>25976</xdr:rowOff>
+      <xdr:rowOff>34637</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Rectangle: Beveled 2">
+        <xdr:cNvPr id="4" name="Rectangle: Beveled 3">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87C83F66-3350-459E-83CB-7B18E6A109BD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{061FE375-5198-4EB7-8E11-FDA27B191B53}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -460,80 +384,56 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="225136" y="3177886"/>
-          <a:ext cx="2052204" cy="355022"/>
+          <a:off x="233795" y="3108614"/>
+          <a:ext cx="2078182" cy="432955"/>
         </a:xfrm>
         <a:prstGeom prst="bevel">
-          <a:avLst/>
+          <a:avLst>
+            <a:gd name="adj" fmla="val 0"/>
+          </a:avLst>
         </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="0">
-          <a:schemeClr val="accent3"/>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
         </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent3"/>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
         </a:fillRef>
-        <a:effectRef idx="3">
-          <a:schemeClr val="accent3"/>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="lt1"/>
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr algn="l"/>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="ar-EG" sz="1100"/>
+            <a:t>أنقر</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ar-EG" sz="1100" baseline="0"/>
+            <a:t> هنا لإضافة مبنى </a:t>
+          </a:r>
           <a:endParaRPr lang="en-IN" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>103910</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>86591</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1250057</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>188724</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE6530FB-76F6-4ABE-9E72-01EDEDA261E0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="658092" y="3212523"/>
-          <a:ext cx="1146147" cy="292633"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -582,7 +482,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -634,7 +534,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -835,50 +735,50 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.265625" customWidth="1"/>
-    <col min="2" max="2" width="32.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="69.1328125" customWidth="1"/>
-    <col min="4" max="4" width="21.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21">
-      <c r="C1" s="16" t="s">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="C1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="16"/>
-    </row>
-    <row r="2" spans="1:9" ht="60" customHeight="1">
+      <c r="D1" s="14"/>
+    </row>
+    <row r="2" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="11"/>
-      <c r="C2" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="C2" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>5</v>
@@ -887,9 +787,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>6</v>
@@ -898,92 +798,92 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E6" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" s="10">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" s="10">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" s="10">
         <v>6</v>
       </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C10" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="E10" s="10">
         <v>7</v>
       </c>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="20"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="17"/>
+      <c r="C11" s="18"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="3"/>
       <c r="C12" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1">
-      <c r="B13" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="17"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="15"/>
       <c r="D13" s="8" t="s">
         <v>0</v>
       </c>
@@ -993,11 +893,11 @@
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
     </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1">
-      <c r="B14" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="17"/>
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="15"/>
       <c r="D14" s="8" t="s">
         <v>1</v>
       </c>
@@ -1007,11 +907,11 @@
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1">
-      <c r="B15" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="17"/>
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="15"/>
       <c r="D15" s="9" t="s">
         <v>2</v>
       </c>
@@ -1021,11 +921,11 @@
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1">
-      <c r="B16" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="17"/>
+    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="15"/>
       <c r="D16" s="9" t="s">
         <v>3</v>
       </c>
@@ -1036,7 +936,6 @@
       <c r="I16" s="7"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="ZOcwxKUyFs0RZTeKMu4ILW755GHrKuHecvxEKyRTU1kmTuLUZg+ttOT5mOR9sEmVMDA4IhMl/R0HJHll5/1YpA==" saltValue="QWCvI93jNG4Jffqb7/p44g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="8">
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C1:D1"/>
@@ -1054,143 +953,50 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.59765625" customWidth="1"/>
-    <col min="2" max="2" width="15.73046875" customWidth="1"/>
+    <col min="1" max="1" width="29.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="51" customWidth="1"/>
-    <col min="4" max="4" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="32.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="14" customFormat="1" hidden="1">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3">
-        <v>456</v>
-      </c>
-      <c r="E3">
-        <v>501234567</v>
-      </c>
-      <c r="F3">
-        <v>506328788</v>
-      </c>
-      <c r="G3" s="22">
-        <v>43565</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4">
-        <v>678</v>
-      </c>
-      <c r="E4">
-        <v>508738732</v>
-      </c>
-      <c r="F4">
-        <v>557838388</v>
-      </c>
-      <c r="G4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="22.15">
-      <c r="A5" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5">
-        <v>456</v>
-      </c>
-      <c r="E5">
-        <v>505989993</v>
-      </c>
-      <c r="F5">
-        <v>587373737</v>
-      </c>
-      <c r="G5" t="s">
-        <v>47</v>
-      </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="F7ZiKjsQgLIYplrlwYkeNWsoQ2NHf7MA8HkVefiJf9TQv3dBNtsVBXQUyip4rU+pSHDt6eU/eNM+7zUshiUh3g==" saltValue="zUiuwqxIGlNE46aUTgtkKw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
-    <protectedRange sqref="A3:G1048576" name="BuildingLists"/>
+    <protectedRange sqref="A2:G1048576" name="BuildingLists"/>
   </protectedRanges>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Creating a webservice for admin dashboard
</commit_message>
<xml_diff>
--- a/upload/نموذج أضافة المبانى -أمان.xlsx
+++ b/upload/نموذج أضافة المبانى -أمان.xlsx
@@ -435,9 +435,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1877760</xdr:colOff>
+      <xdr:colOff>1877040</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>55800</xdr:rowOff>
+      <xdr:rowOff>55080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -451,7 +451,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="346320" y="379080"/>
-          <a:ext cx="2266560" cy="705240"/>
+          <a:ext cx="2265840" cy="704520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -472,9 +472,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1722600</xdr:colOff>
+      <xdr:colOff>1721880</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>25560</xdr:rowOff>
+      <xdr:rowOff>24840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -486,13 +486,14 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="225000" y="3080520"/>
-          <a:ext cx="2232720" cy="354960"/>
+          <a:ext cx="2232000" cy="354240"/>
         </a:xfrm>
         <a:prstGeom prst="bevel">
           <a:avLst>
             <a:gd name="adj" fmla="val 12500"/>
           </a:avLst>
         </a:prstGeom>
+        <a:noFill/>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -528,9 +529,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1249920</xdr:colOff>
+      <xdr:colOff>1249200</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>188640</xdr:rowOff>
+      <xdr:rowOff>187920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -544,7 +545,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="839160" y="3115440"/>
-          <a:ext cx="1145880" cy="292320"/>
+          <a:ext cx="1145160" cy="291600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -567,7 +568,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="A3:G5 C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="A3:G4 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -793,8 +794,8 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E2" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3:G5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="A3:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>